<commit_message>
bab 4 bagian gua clear
</commit_message>
<xml_diff>
--- a/data_mentah.xlsx
+++ b/data_mentah.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Project\Niken\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD43A6F-E6C4-4102-92C1-F3D15E75B480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
-    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
-    <sheet r:id="rId3" sheetId="3" name="Sheet3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="369">
   <si>
     <t>No</t>
   </si>
@@ -1114,14 +1120,22 @@
   </si>
   <si>
     <t>4 Bulan</t>
+  </si>
+  <si>
+    <t>Ketepatan</t>
+  </si>
+  <si>
+    <t>Kreatifitasi</t>
+  </si>
+  <si>
+    <t>Waktu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1142,8 +1156,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1152,16 +1185,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd7e4bd"/>
+        <fgColor rgb="FFD7E4BD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1174,7 +1213,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -1210,7 +1249,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1223,16 +1262,64 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1240,68 +1327,92 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1312,10 +1423,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1353,71 +1464,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1445,7 +1556,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1468,11 +1579,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1481,13 +1592,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1497,7 +1608,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1506,7 +1617,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1515,7 +1626,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1523,10 +1634,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1591,40 +1702,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:U113"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="8.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="32.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="38.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="16" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="17" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="14" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="13" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="13" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="13" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="6.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="48">
+    <row r="1" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1689,14 +1800,14 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1723,10 +1834,10 @@
       <c r="K2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>34954</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="10">
         <v>44440</v>
       </c>
       <c r="N2" s="8" t="s">
@@ -1754,14 +1865,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1788,10 +1899,10 @@
       <c r="K3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <v>35282</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>44440</v>
       </c>
       <c r="N3" s="8" t="s">
@@ -1819,14 +1930,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -1853,10 +1964,10 @@
       <c r="K4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>33176</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="10">
         <v>44440</v>
       </c>
       <c r="N4" s="8" t="s">
@@ -1884,14 +1995,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -1918,10 +2029,10 @@
       <c r="K5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="9">
         <v>33417</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <v>44440</v>
       </c>
       <c r="N5" s="8" t="s">
@@ -1949,14 +2060,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1983,10 +2094,10 @@
       <c r="K6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>35616</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <v>44440</v>
       </c>
       <c r="N6" s="8" t="s">
@@ -2014,14 +2125,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -2048,10 +2159,10 @@
       <c r="K7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="9">
         <v>33370</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="10">
         <v>44440</v>
       </c>
       <c r="N7" s="8" t="s">
@@ -2079,14 +2190,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -2113,10 +2224,10 @@
       <c r="K8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <v>35242</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="10">
         <v>44440</v>
       </c>
       <c r="N8" s="8" t="s">
@@ -2144,14 +2255,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -2178,10 +2289,10 @@
       <c r="K9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="9">
         <v>33921</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>44440</v>
       </c>
       <c r="N9" s="8" t="s">
@@ -2209,14 +2320,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -2243,10 +2354,10 @@
       <c r="K10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <v>35694</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="10">
         <v>44440</v>
       </c>
       <c r="N10" s="8" t="s">
@@ -2274,14 +2385,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s">
         <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -2308,10 +2419,10 @@
       <c r="K11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <v>37190</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>44501</v>
       </c>
       <c r="N11" s="8" t="s">
@@ -2339,14 +2450,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" t="s">
         <v>66</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -2373,10 +2484,10 @@
       <c r="K12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <v>34241</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <v>44743</v>
       </c>
       <c r="N12" s="8" t="s">
@@ -2404,14 +2515,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -2438,10 +2549,10 @@
       <c r="K13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="9">
         <v>35342</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="10">
         <v>43831</v>
       </c>
       <c r="N13" s="8" t="s">
@@ -2469,14 +2580,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" t="s">
         <v>75</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -2503,10 +2614,10 @@
       <c r="K14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <v>24822</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="10">
         <v>33721</v>
       </c>
       <c r="N14" s="8" t="s">
@@ -2534,14 +2645,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" t="s">
         <v>81</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -2568,10 +2679,10 @@
       <c r="K15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="9">
         <v>25026</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="10">
         <v>34171</v>
       </c>
       <c r="N15" s="8" t="s">
@@ -2599,14 +2710,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" t="s">
         <v>88</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -2633,10 +2744,10 @@
       <c r="K16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="9">
         <v>25020</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="10">
         <v>31779</v>
       </c>
       <c r="N16" s="8" t="s">
@@ -2664,14 +2775,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -2698,10 +2809,10 @@
       <c r="K17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="9">
         <v>24990</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="10">
         <v>32437</v>
       </c>
       <c r="N17" s="8" t="s">
@@ -2729,14 +2840,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" t="s">
         <v>101</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -2763,10 +2874,10 @@
       <c r="K18" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="9">
         <v>25182</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="10">
         <v>32772</v>
       </c>
       <c r="N18" s="8" t="s">
@@ -2794,14 +2905,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" t="s">
         <v>106</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -2828,10 +2939,10 @@
       <c r="K19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="9">
         <v>25175</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="10">
         <v>33075</v>
       </c>
       <c r="N19" s="8" t="s">
@@ -2859,14 +2970,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" t="s">
         <v>110</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -2893,10 +3004,10 @@
       <c r="K20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>26121</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="10">
         <v>33745</v>
       </c>
       <c r="N20" s="8" t="s">
@@ -2924,14 +3035,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" t="s">
         <v>113</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -2958,10 +3069,10 @@
       <c r="K21" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="9">
         <v>24969</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M21" s="10">
         <v>35329</v>
       </c>
       <c r="N21" s="8" t="s">
@@ -2989,14 +3100,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" t="s">
         <v>115</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -3023,10 +3134,10 @@
       <c r="K22" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="9">
         <v>25187</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="10">
         <v>35602</v>
       </c>
       <c r="N22" s="8" t="s">
@@ -3054,14 +3165,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" t="s">
         <v>117</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -3088,10 +3199,10 @@
       <c r="K23" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="9">
         <v>24971</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="10">
         <v>35952</v>
       </c>
       <c r="N23" s="8" t="s">
@@ -3119,14 +3230,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" t="s">
         <v>121</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -3153,10 +3264,10 @@
       <c r="K24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="9">
         <v>25294</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="10">
         <v>33868</v>
       </c>
       <c r="N24" s="8" t="s">
@@ -3184,14 +3295,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" t="s">
         <v>124</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -3218,10 +3329,10 @@
       <c r="K25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="9">
         <v>25513</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="10">
         <v>33776</v>
       </c>
       <c r="N25" s="8" t="s">
@@ -3249,14 +3360,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="8" t="s">
@@ -3283,10 +3394,10 @@
       <c r="K26" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="9">
         <v>25399</v>
       </c>
-      <c r="M26" s="11">
+      <c r="M26" s="10">
         <v>33973</v>
       </c>
       <c r="N26" s="8" t="s">
@@ -3314,14 +3425,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row r="27" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" t="s">
         <v>129</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -3348,10 +3459,10 @@
       <c r="K27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27" s="9">
         <v>25385</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="10">
         <v>34477</v>
       </c>
       <c r="N27" s="8" t="s">
@@ -3379,14 +3490,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row r="28" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" t="s">
         <v>133</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -3413,10 +3524,10 @@
       <c r="K28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="9">
         <v>25418</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M28" s="10">
         <v>35065</v>
       </c>
       <c r="N28" s="8" t="s">
@@ -3444,14 +3555,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row r="29" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" t="s">
         <v>138</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -3478,10 +3589,10 @@
       <c r="K29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="9">
         <v>25271</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="10">
         <v>35967</v>
       </c>
       <c r="N29" s="8" t="s">
@@ -3509,14 +3620,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" t="s">
         <v>140</v>
       </c>
       <c r="D30" s="8" t="s">
@@ -3543,10 +3654,10 @@
       <c r="K30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="9">
         <v>25544</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="10">
         <v>35510</v>
       </c>
       <c r="N30" s="8" t="s">
@@ -3574,14 +3685,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" t="s">
         <v>143</v>
       </c>
       <c r="D31" s="8" t="s">
@@ -3608,10 +3719,10 @@
       <c r="K31" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="9">
         <v>25297</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="10">
         <v>36393</v>
       </c>
       <c r="N31" s="8" t="s">
@@ -3639,14 +3750,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" t="s">
         <v>146</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -3673,10 +3784,10 @@
       <c r="K32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="9">
         <v>25433</v>
       </c>
-      <c r="M32" s="11">
+      <c r="M32" s="10">
         <v>36424</v>
       </c>
       <c r="N32" s="8" t="s">
@@ -3704,14 +3815,14 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" t="s">
         <v>148</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -3738,10 +3849,10 @@
       <c r="K33" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33" s="9">
         <v>25537</v>
       </c>
-      <c r="M33" s="11">
+      <c r="M33" s="10">
         <v>36667</v>
       </c>
       <c r="N33" s="8" t="s">
@@ -3769,14 +3880,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" t="s">
         <v>151</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -3803,10 +3914,10 @@
       <c r="K34" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="9">
         <v>25682</v>
       </c>
-      <c r="M34" s="11">
+      <c r="M34" s="10">
         <v>32687</v>
       </c>
       <c r="N34" s="8" t="s">
@@ -3834,14 +3945,14 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row r="35" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" t="s">
         <v>155</v>
       </c>
       <c r="D35" s="8" t="s">
@@ -3868,10 +3979,10 @@
       <c r="K35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="9">
         <v>25624</v>
       </c>
-      <c r="M35" s="11">
+      <c r="M35" s="10">
         <v>33456</v>
       </c>
       <c r="N35" s="8" t="s">
@@ -3899,14 +4010,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row r="36" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" t="s">
         <v>157</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -3933,10 +4044,10 @@
       <c r="K36" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L36" s="9">
         <v>25637</v>
       </c>
-      <c r="M36" s="11">
+      <c r="M36" s="10">
         <v>35602</v>
       </c>
       <c r="N36" s="8" t="s">
@@ -3964,14 +4075,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" t="s">
         <v>159</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -3998,10 +4109,10 @@
       <c r="K37" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L37" s="9">
         <v>25786</v>
       </c>
-      <c r="M37" s="11">
+      <c r="M37" s="10">
         <v>35510</v>
       </c>
       <c r="N37" s="8" t="s">
@@ -4029,14 +4140,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row r="38" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" t="s">
         <v>161</v>
       </c>
       <c r="D38" s="8" t="s">
@@ -4063,10 +4174,10 @@
       <c r="K38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="9">
         <v>25885</v>
       </c>
-      <c r="M38" s="11">
+      <c r="M38" s="10">
         <v>36256</v>
       </c>
       <c r="N38" s="8" t="s">
@@ -4094,14 +4205,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" t="s">
         <v>163</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -4128,10 +4239,10 @@
       <c r="K39" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="9">
         <v>25851</v>
       </c>
-      <c r="M39" s="11">
+      <c r="M39" s="10">
         <v>36606</v>
       </c>
       <c r="N39" s="8" t="s">
@@ -4159,14 +4270,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" t="s">
         <v>165</v>
       </c>
       <c r="D40" s="8" t="s">
@@ -4193,10 +4304,10 @@
       <c r="K40" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L40" s="10">
+      <c r="L40" s="9">
         <v>26279</v>
       </c>
-      <c r="M40" s="11">
+      <c r="M40" s="10">
         <v>32560</v>
       </c>
       <c r="N40" s="8" t="s">
@@ -4224,14 +4335,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row r="41" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" t="s">
         <v>168</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -4258,10 +4369,10 @@
       <c r="K41" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L41" s="10">
+      <c r="L41" s="9">
         <v>26266</v>
       </c>
-      <c r="M41" s="11">
+      <c r="M41" s="10">
         <v>33929</v>
       </c>
       <c r="N41" s="8" t="s">
@@ -4289,14 +4400,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row r="42" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" t="s">
         <v>170</v>
       </c>
       <c r="D42" s="8" t="s">
@@ -4323,10 +4434,10 @@
       <c r="K42" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L42" s="10">
+      <c r="L42" s="9">
         <v>26278</v>
       </c>
-      <c r="M42" s="11">
+      <c r="M42" s="10">
         <v>33745</v>
       </c>
       <c r="N42" s="8" t="s">
@@ -4354,14 +4465,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+    <row r="43" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" t="s">
         <v>173</v>
       </c>
       <c r="D43" s="8" t="s">
@@ -4388,10 +4499,10 @@
       <c r="K43" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L43" s="10">
+      <c r="L43" s="9">
         <v>25938</v>
       </c>
-      <c r="M43" s="11">
+      <c r="M43" s="10">
         <v>34400</v>
       </c>
       <c r="N43" s="8" t="s">
@@ -4419,14 +4530,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row r="44" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" t="s">
         <v>175</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -4453,10 +4564,10 @@
       <c r="K44" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L44" s="10">
+      <c r="L44" s="9">
         <v>26190</v>
       </c>
-      <c r="M44" s="11">
+      <c r="M44" s="10">
         <v>34400</v>
       </c>
       <c r="N44" s="8" t="s">
@@ -4484,14 +4595,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row r="45" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" t="s">
         <v>177</v>
       </c>
       <c r="D45" s="8" t="s">
@@ -4518,10 +4629,10 @@
       <c r="K45" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L45" s="10">
+      <c r="L45" s="9">
         <v>26079</v>
       </c>
-      <c r="M45" s="11">
+      <c r="M45" s="10">
         <v>34810</v>
       </c>
       <c r="N45" s="8" t="s">
@@ -4549,14 +4660,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row r="46" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" t="s">
         <v>181</v>
       </c>
       <c r="D46" s="8" t="s">
@@ -4583,10 +4694,10 @@
       <c r="K46" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L46" s="10">
+      <c r="L46" s="9">
         <v>26206</v>
       </c>
-      <c r="M46" s="11">
+      <c r="M46" s="10">
         <v>34912</v>
       </c>
       <c r="N46" s="8" t="s">
@@ -4614,14 +4725,14 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row r="47" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" t="s">
         <v>183</v>
       </c>
       <c r="D47" s="8" t="s">
@@ -4648,10 +4759,10 @@
       <c r="K47" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L47" s="10">
+      <c r="L47" s="9">
         <v>26272</v>
       </c>
-      <c r="M47" s="11">
+      <c r="M47" s="10">
         <v>35065</v>
       </c>
       <c r="N47" s="8" t="s">
@@ -4679,14 +4790,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row r="48" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" t="s">
         <v>185</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -4713,10 +4824,10 @@
       <c r="K48" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L48" s="10">
+      <c r="L48" s="9">
         <v>25997</v>
       </c>
-      <c r="M48" s="11">
+      <c r="M48" s="10">
         <v>35436</v>
       </c>
       <c r="N48" s="8" t="s">
@@ -4744,14 +4855,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row r="49" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" t="s">
         <v>188</v>
       </c>
       <c r="D49" s="8" t="s">
@@ -4778,10 +4889,10 @@
       <c r="K49" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L49" s="10">
+      <c r="L49" s="9">
         <v>26279</v>
       </c>
-      <c r="M49" s="11">
+      <c r="M49" s="10">
         <v>35602</v>
       </c>
       <c r="N49" s="8" t="s">
@@ -4809,14 +4920,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+    <row r="50" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" t="s">
         <v>190</v>
       </c>
       <c r="D50" s="8" t="s">
@@ -4843,10 +4954,10 @@
       <c r="K50" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L50" s="10">
+      <c r="L50" s="9">
         <v>26292</v>
       </c>
-      <c r="M50" s="11">
+      <c r="M50" s="10">
         <v>35947</v>
       </c>
       <c r="N50" s="8" t="s">
@@ -4874,14 +4985,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row r="51" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" t="s">
         <v>194</v>
       </c>
       <c r="D51" s="8" t="s">
@@ -4908,10 +5019,10 @@
       <c r="K51" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L51" s="10">
+      <c r="L51" s="9">
         <v>26315</v>
       </c>
-      <c r="M51" s="11">
+      <c r="M51" s="10">
         <v>32772</v>
       </c>
       <c r="N51" s="8" t="s">
@@ -4939,14 +5050,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row r="52" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" t="s">
         <v>198</v>
       </c>
       <c r="D52" s="8" t="s">
@@ -4973,10 +5084,10 @@
       <c r="K52" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L52" s="10">
+      <c r="L52" s="9">
         <v>26413</v>
       </c>
-      <c r="M52" s="11">
+      <c r="M52" s="10">
         <v>33137</v>
       </c>
       <c r="N52" s="8" t="s">
@@ -5004,14 +5115,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row r="53" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" t="s">
         <v>200</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -5038,10 +5149,10 @@
       <c r="K53" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L53" s="10">
+      <c r="L53" s="9">
         <v>26654</v>
       </c>
-      <c r="M53" s="11">
+      <c r="M53" s="10">
         <v>32984</v>
       </c>
       <c r="N53" s="8" t="s">
@@ -5069,14 +5180,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row r="54" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" t="s">
         <v>202</v>
       </c>
       <c r="D54" s="8" t="s">
@@ -5103,10 +5214,10 @@
       <c r="K54" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L54" s="10">
+      <c r="L54" s="9">
         <v>26395</v>
       </c>
-      <c r="M54" s="11">
+      <c r="M54" s="10">
         <v>33776</v>
       </c>
       <c r="N54" s="8" t="s">
@@ -5134,14 +5245,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+    <row r="55" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="8" t="s">
@@ -5168,10 +5279,10 @@
       <c r="K55" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L55" s="10">
+      <c r="L55" s="9">
         <v>26475</v>
       </c>
-      <c r="M55" s="11">
+      <c r="M55" s="10">
         <v>33929</v>
       </c>
       <c r="N55" s="8" t="s">
@@ -5199,14 +5310,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row r="56" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="8" t="s">
@@ -5233,10 +5344,10 @@
       <c r="K56" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L56" s="10">
+      <c r="L56" s="9">
         <v>26573</v>
       </c>
-      <c r="M56" s="11">
+      <c r="M56" s="10">
         <v>33898</v>
       </c>
       <c r="N56" s="8" t="s">
@@ -5264,14 +5375,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+    <row r="57" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" t="s">
         <v>211</v>
       </c>
       <c r="D57" s="8" t="s">
@@ -5298,10 +5409,10 @@
       <c r="K57" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L57" s="10">
+      <c r="L57" s="9">
         <v>26317</v>
       </c>
-      <c r="M57" s="11">
+      <c r="M57" s="10">
         <v>34751</v>
       </c>
       <c r="N57" s="8" t="s">
@@ -5329,14 +5440,14 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row r="58" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" t="s">
         <v>214</v>
       </c>
       <c r="D58" s="8" t="s">
@@ -5363,10 +5474,10 @@
       <c r="K58" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L58" s="10">
+      <c r="L58" s="9">
         <v>26536</v>
       </c>
-      <c r="M58" s="11">
+      <c r="M58" s="10">
         <v>35237</v>
       </c>
       <c r="N58" s="8" t="s">
@@ -5394,14 +5505,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+    <row r="59" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" t="s">
         <v>216</v>
       </c>
       <c r="D59" s="8" t="s">
@@ -5428,10 +5539,10 @@
       <c r="K59" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L59" s="10">
+      <c r="L59" s="9">
         <v>26371</v>
       </c>
-      <c r="M59" s="11">
+      <c r="M59" s="10">
         <v>35436</v>
       </c>
       <c r="N59" s="8" t="s">
@@ -5459,14 +5570,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row r="60" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" t="s">
         <v>218</v>
       </c>
       <c r="D60" s="8" t="s">
@@ -5493,10 +5604,10 @@
       <c r="K60" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L60" s="10">
+      <c r="L60" s="9">
         <v>26547</v>
       </c>
-      <c r="M60" s="11">
+      <c r="M60" s="10">
         <v>35602</v>
       </c>
       <c r="N60" s="8" t="s">
@@ -5524,14 +5635,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+    <row r="61" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" t="s">
         <v>221</v>
       </c>
       <c r="D61" s="8" t="s">
@@ -5558,10 +5669,10 @@
       <c r="K61" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L61" s="10">
+      <c r="L61" s="9">
         <v>26462</v>
       </c>
-      <c r="M61" s="11">
+      <c r="M61" s="10">
         <v>35967</v>
       </c>
       <c r="N61" s="8" t="s">
@@ -5589,14 +5700,14 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+    <row r="62" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" t="s">
         <v>223</v>
       </c>
       <c r="D62" s="8" t="s">
@@ -5623,10 +5734,10 @@
       <c r="K62" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L62" s="10">
+      <c r="L62" s="9">
         <v>26651</v>
       </c>
-      <c r="M62" s="11">
+      <c r="M62" s="10">
         <v>35906</v>
       </c>
       <c r="N62" s="8" t="s">
@@ -5654,14 +5765,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+    <row r="63" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" t="s">
         <v>225</v>
       </c>
       <c r="D63" s="8" t="s">
@@ -5688,10 +5799,10 @@
       <c r="K63" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L63" s="10">
+      <c r="L63" s="9">
         <v>26759</v>
       </c>
-      <c r="M63" s="11">
+      <c r="M63" s="10">
         <v>34445</v>
       </c>
       <c r="N63" s="8" t="s">
@@ -5719,14 +5830,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+    <row r="64" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" t="s">
         <v>229</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -5753,10 +5864,10 @@
       <c r="K64" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L64" s="10">
+      <c r="L64" s="9">
         <v>26979</v>
       </c>
-      <c r="M64" s="11">
+      <c r="M64" s="10">
         <v>35436</v>
       </c>
       <c r="N64" s="8" t="s">
@@ -5784,14 +5895,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+    <row r="65" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>64</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" t="s">
         <v>231</v>
       </c>
       <c r="D65" s="8" t="s">
@@ -5818,10 +5929,10 @@
       <c r="K65" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L65" s="10">
+      <c r="L65" s="9">
         <v>26778</v>
       </c>
-      <c r="M65" s="11">
+      <c r="M65" s="10">
         <v>35875</v>
       </c>
       <c r="N65" s="8" t="s">
@@ -5849,14 +5960,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+    <row r="66" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" t="s">
         <v>233</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -5883,10 +5994,10 @@
       <c r="K66" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L66" s="10">
+      <c r="L66" s="9">
         <v>26979</v>
       </c>
-      <c r="M66" s="11">
+      <c r="M66" s="10">
         <v>36181</v>
       </c>
       <c r="N66" s="8" t="s">
@@ -5914,14 +6025,14 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+    <row r="67" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>66</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" t="s">
         <v>236</v>
       </c>
       <c r="D67" s="8" t="s">
@@ -5948,10 +6059,10 @@
       <c r="K67" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L67" s="10">
+      <c r="L67" s="9">
         <v>27166</v>
       </c>
-      <c r="M67" s="11">
+      <c r="M67" s="10">
         <v>33973</v>
       </c>
       <c r="N67" s="8" t="s">
@@ -5979,14 +6090,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
+    <row r="68" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" t="s">
         <v>239</v>
       </c>
       <c r="D68" s="8" t="s">
@@ -6013,10 +6124,10 @@
       <c r="K68" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L68" s="10">
+      <c r="L68" s="9">
         <v>27085</v>
       </c>
-      <c r="M68" s="11">
+      <c r="M68" s="10">
         <v>34871</v>
       </c>
       <c r="N68" s="8" t="s">
@@ -6044,14 +6155,14 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
+    <row r="69" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>68</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" t="s">
         <v>241</v>
       </c>
       <c r="D69" s="8" t="s">
@@ -6078,10 +6189,10 @@
       <c r="K69" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L69" s="10">
+      <c r="L69" s="9">
         <v>27213</v>
       </c>
-      <c r="M69" s="11">
+      <c r="M69" s="10">
         <v>34871</v>
       </c>
       <c r="N69" s="8" t="s">
@@ -6109,14 +6220,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+    <row r="70" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" t="s">
         <v>244</v>
       </c>
       <c r="D70" s="8" t="s">
@@ -6143,10 +6254,10 @@
       <c r="K70" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L70" s="10">
+      <c r="L70" s="9">
         <v>27096</v>
       </c>
-      <c r="M70" s="11">
+      <c r="M70" s="10">
         <v>35268</v>
       </c>
       <c r="N70" s="8" t="s">
@@ -6174,14 +6285,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+    <row r="71" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>70</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" t="s">
         <v>247</v>
       </c>
       <c r="D71" s="8" t="s">
@@ -6208,10 +6319,10 @@
       <c r="K71" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L71" s="10">
+      <c r="L71" s="9">
         <v>27286</v>
       </c>
-      <c r="M71" s="11">
+      <c r="M71" s="10">
         <v>35967</v>
       </c>
       <c r="N71" s="8" t="s">
@@ -6239,14 +6350,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+    <row r="72" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>71</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" t="s">
         <v>249</v>
       </c>
       <c r="D72" s="8" t="s">
@@ -6273,10 +6384,10 @@
       <c r="K72" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L72" s="10">
+      <c r="L72" s="9">
         <v>27271</v>
       </c>
-      <c r="M72" s="11">
+      <c r="M72" s="10">
         <v>36393</v>
       </c>
       <c r="N72" s="8" t="s">
@@ -6304,14 +6415,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
+    <row r="73" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>72</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" t="s">
         <v>252</v>
       </c>
       <c r="D73" s="8" t="s">
@@ -6338,10 +6449,10 @@
       <c r="K73" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L73" s="10">
+      <c r="L73" s="9">
         <v>27467</v>
       </c>
-      <c r="M73" s="11">
+      <c r="M73" s="10">
         <v>34400</v>
       </c>
       <c r="N73" s="8" t="s">
@@ -6369,14 +6480,14 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
+    <row r="74" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>73</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" t="s">
         <v>255</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -6403,10 +6514,10 @@
       <c r="K74" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L74" s="10">
+      <c r="L74" s="9">
         <v>27494</v>
       </c>
-      <c r="M74" s="11">
+      <c r="M74" s="10">
         <v>34751</v>
       </c>
       <c r="N74" s="8" t="s">
@@ -6434,14 +6545,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+    <row r="75" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>74</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" t="s">
         <v>258</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -6468,10 +6579,10 @@
       <c r="K75" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L75" s="10">
+      <c r="L75" s="9">
         <v>27528</v>
       </c>
-      <c r="M75" s="11">
+      <c r="M75" s="10">
         <v>35065</v>
       </c>
       <c r="N75" s="8" t="s">
@@ -6499,14 +6610,14 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+    <row r="76" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>75</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" t="s">
         <v>261</v>
       </c>
       <c r="D76" s="8" t="s">
@@ -6533,10 +6644,10 @@
       <c r="K76" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L76" s="10">
+      <c r="L76" s="9">
         <v>27525</v>
       </c>
-      <c r="M76" s="11">
+      <c r="M76" s="10">
         <v>35541</v>
       </c>
       <c r="N76" s="8" t="s">
@@ -6564,14 +6675,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
+    <row r="77" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>76</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" t="s">
         <v>264</v>
       </c>
       <c r="D77" s="8" t="s">
@@ -6598,10 +6709,10 @@
       <c r="K77" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L77" s="10">
+      <c r="L77" s="9">
         <v>27616</v>
       </c>
-      <c r="M77" s="11">
+      <c r="M77" s="10">
         <v>35510</v>
       </c>
       <c r="N77" s="8" t="s">
@@ -6629,14 +6740,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
+    <row r="78" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>77</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" t="s">
         <v>266</v>
       </c>
       <c r="D78" s="8" t="s">
@@ -6663,10 +6774,10 @@
       <c r="K78" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L78" s="10">
+      <c r="L78" s="9">
         <v>27515</v>
       </c>
-      <c r="M78" s="11">
+      <c r="M78" s="10">
         <v>35967</v>
       </c>
       <c r="N78" s="8" t="s">
@@ -6694,14 +6805,14 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
+    <row r="79" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>78</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" t="s">
         <v>268</v>
       </c>
       <c r="D79" s="8" t="s">
@@ -6728,10 +6839,10 @@
       <c r="K79" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L79" s="10">
+      <c r="L79" s="9">
         <v>25333</v>
       </c>
-      <c r="M79" s="11">
+      <c r="M79" s="10">
         <v>34033</v>
       </c>
       <c r="N79" s="8" t="s">
@@ -6759,14 +6870,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
+    <row r="80" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="C80" t="s">
         <v>270</v>
       </c>
       <c r="D80" s="8" t="s">
@@ -6793,10 +6904,10 @@
       <c r="K80" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L80" s="10">
+      <c r="L80" s="9">
         <v>27399</v>
       </c>
-      <c r="M80" s="11">
+      <c r="M80" s="10">
         <v>36181</v>
       </c>
       <c r="N80" s="8" t="s">
@@ -6824,14 +6935,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
+    <row r="81" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" t="s">
         <v>273</v>
       </c>
       <c r="D81" s="8" t="s">
@@ -6858,10 +6969,10 @@
       <c r="K81" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L81" s="10">
+      <c r="L81" s="9">
         <v>27942</v>
       </c>
-      <c r="M81" s="11">
+      <c r="M81" s="10">
         <v>34080</v>
       </c>
       <c r="N81" s="8" t="s">
@@ -6889,14 +7000,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
+    <row r="82" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" t="s">
         <v>277</v>
       </c>
       <c r="D82" s="8" t="s">
@@ -6923,10 +7034,10 @@
       <c r="K82" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L82" s="10">
+      <c r="L82" s="9">
         <v>27857</v>
       </c>
-      <c r="M82" s="11">
+      <c r="M82" s="10">
         <v>35329</v>
       </c>
       <c r="N82" s="8" t="s">
@@ -6954,14 +7065,14 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
+    <row r="83" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" t="s">
         <v>279</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -6988,10 +7099,10 @@
       <c r="K83" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L83" s="10">
+      <c r="L83" s="9">
         <v>27948</v>
       </c>
-      <c r="M83" s="11">
+      <c r="M83" s="10">
         <v>35176</v>
       </c>
       <c r="N83" s="8" t="s">
@@ -7019,14 +7130,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
+    <row r="84" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" t="s">
         <v>281</v>
       </c>
       <c r="D84" s="8" t="s">
@@ -7053,10 +7164,10 @@
       <c r="K84" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L84" s="10">
+      <c r="L84" s="9">
         <v>27812</v>
       </c>
-      <c r="M84" s="11">
+      <c r="M84" s="10">
         <v>35510</v>
       </c>
       <c r="N84" s="8" t="s">
@@ -7084,14 +7195,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+    <row r="85" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="C85" s="9" t="s">
+      <c r="C85" t="s">
         <v>283</v>
       </c>
       <c r="D85" s="8" t="s">
@@ -7118,10 +7229,10 @@
       <c r="K85" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L85" s="10">
+      <c r="L85" s="9">
         <v>27800</v>
       </c>
-      <c r="M85" s="11">
+      <c r="M85" s="10">
         <v>35510</v>
       </c>
       <c r="N85" s="8" t="s">
@@ -7149,14 +7260,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
+    <row r="86" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" t="s">
         <v>286</v>
       </c>
       <c r="D86" s="8" t="s">
@@ -7183,10 +7294,10 @@
       <c r="K86" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L86" s="10">
+      <c r="L86" s="9">
         <v>27927</v>
       </c>
-      <c r="M86" s="11">
+      <c r="M86" s="10">
         <v>35510</v>
       </c>
       <c r="N86" s="8" t="s">
@@ -7214,14 +7325,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+    <row r="87" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="C87" t="s">
         <v>289</v>
       </c>
       <c r="D87" s="8" t="s">
@@ -7248,10 +7359,10 @@
       <c r="K87" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L87" s="10">
+      <c r="L87" s="9">
         <v>27899</v>
       </c>
-      <c r="M87" s="11">
+      <c r="M87" s="10">
         <v>35875</v>
       </c>
       <c r="N87" s="8" t="s">
@@ -7279,14 +7390,14 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
+    <row r="88" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" t="s">
         <v>291</v>
       </c>
       <c r="D88" s="8" t="s">
@@ -7313,10 +7424,10 @@
       <c r="K88" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L88" s="10">
+      <c r="L88" s="9">
         <v>27930</v>
       </c>
-      <c r="M88" s="11">
+      <c r="M88" s="10">
         <v>35847</v>
       </c>
       <c r="N88" s="8" t="s">
@@ -7344,14 +7455,14 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
+    <row r="89" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" t="s">
         <v>293</v>
       </c>
       <c r="D89" s="8" t="s">
@@ -7378,10 +7489,10 @@
       <c r="K89" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L89" s="10">
+      <c r="L89" s="9">
         <v>27785</v>
       </c>
-      <c r="M89" s="11">
+      <c r="M89" s="10">
         <v>36393</v>
       </c>
       <c r="N89" s="8" t="s">
@@ -7409,14 +7520,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
+    <row r="90" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C90" t="s">
         <v>296</v>
       </c>
       <c r="D90" s="8" t="s">
@@ -7443,10 +7554,10 @@
       <c r="K90" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L90" s="10">
+      <c r="L90" s="9">
         <v>28371</v>
       </c>
-      <c r="M90" s="11">
+      <c r="M90" s="10">
         <v>35602</v>
       </c>
       <c r="N90" s="8" t="s">
@@ -7474,14 +7585,14 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
+    <row r="91" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C91" t="s">
         <v>299</v>
       </c>
       <c r="D91" s="8" t="s">
@@ -7508,10 +7619,10 @@
       <c r="K91" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L91" s="10">
+      <c r="L91" s="9">
         <v>28454</v>
       </c>
-      <c r="M91" s="11">
+      <c r="M91" s="10">
         <v>36271</v>
       </c>
       <c r="N91" s="8" t="s">
@@ -7539,14 +7650,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
+    <row r="92" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C92" t="s">
         <v>303</v>
       </c>
       <c r="D92" s="8" t="s">
@@ -7573,10 +7684,10 @@
       <c r="K92" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L92" s="10">
+      <c r="L92" s="9">
         <v>28449</v>
       </c>
-      <c r="M92" s="11">
+      <c r="M92" s="10">
         <v>36606</v>
       </c>
       <c r="N92" s="8" t="s">
@@ -7604,14 +7715,14 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
+    <row r="93" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="C93" s="9" t="s">
+      <c r="C93" t="s">
         <v>306</v>
       </c>
       <c r="D93" s="8" t="s">
@@ -7638,10 +7749,10 @@
       <c r="K93" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L93" s="10">
+      <c r="L93" s="9">
         <v>28503</v>
       </c>
-      <c r="M93" s="11">
+      <c r="M93" s="10">
         <v>35206</v>
       </c>
       <c r="N93" s="8" t="s">
@@ -7669,14 +7780,14 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
+    <row r="94" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" t="s">
         <v>309</v>
       </c>
       <c r="D94" s="8" t="s">
@@ -7703,10 +7814,10 @@
       <c r="K94" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L94" s="10">
+      <c r="L94" s="9">
         <v>28562</v>
       </c>
-      <c r="M94" s="11">
+      <c r="M94" s="10">
         <v>35206</v>
       </c>
       <c r="N94" s="8" t="s">
@@ -7734,14 +7845,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
+    <row r="95" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" t="s">
         <v>312</v>
       </c>
       <c r="D95" s="8" t="s">
@@ -7768,10 +7879,10 @@
       <c r="K95" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L95" s="10">
+      <c r="L95" s="9">
         <v>28672</v>
       </c>
-      <c r="M95" s="11">
+      <c r="M95" s="10">
         <v>35541</v>
       </c>
       <c r="N95" s="8" t="s">
@@ -7799,14 +7910,14 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
+    <row r="96" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C96" t="s">
         <v>314</v>
       </c>
       <c r="D96" s="8" t="s">
@@ -7833,10 +7944,10 @@
       <c r="K96" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L96" s="10">
+      <c r="L96" s="9">
         <v>28588</v>
       </c>
-      <c r="M96" s="11">
+      <c r="M96" s="10">
         <v>35967</v>
       </c>
       <c r="N96" s="8" t="s">
@@ -7864,14 +7975,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
+    <row r="97" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="C97" t="s">
         <v>316</v>
       </c>
       <c r="D97" s="8" t="s">
@@ -7898,10 +8009,10 @@
       <c r="K97" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L97" s="10">
+      <c r="L97" s="9">
         <v>28653</v>
       </c>
-      <c r="M97" s="11">
+      <c r="M97" s="10">
         <v>35816</v>
       </c>
       <c r="N97" s="8" t="s">
@@ -7929,14 +8040,14 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
+    <row r="98" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="C98" t="s">
         <v>318</v>
       </c>
       <c r="D98" s="8" t="s">
@@ -7963,10 +8074,10 @@
       <c r="K98" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L98" s="10">
+      <c r="L98" s="9">
         <v>28562</v>
       </c>
-      <c r="M98" s="11">
+      <c r="M98" s="10">
         <v>36181</v>
       </c>
       <c r="N98" s="8" t="s">
@@ -7994,14 +8105,14 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
+    <row r="99" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" t="s">
         <v>320</v>
       </c>
       <c r="D99" s="8" t="s">
@@ -8028,10 +8139,10 @@
       <c r="K99" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L99" s="10">
+      <c r="L99" s="9">
         <v>28491</v>
       </c>
-      <c r="M99" s="11">
+      <c r="M99" s="10">
         <v>36606</v>
       </c>
       <c r="N99" s="8" t="s">
@@ -8059,14 +8170,14 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
+    <row r="100" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C100" t="s">
         <v>323</v>
       </c>
       <c r="D100" s="8" t="s">
@@ -8093,10 +8204,10 @@
       <c r="K100" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L100" s="10">
+      <c r="L100" s="9">
         <v>28718</v>
       </c>
-      <c r="M100" s="11">
+      <c r="M100" s="10">
         <v>36606</v>
       </c>
       <c r="N100" s="8" t="s">
@@ -8124,14 +8235,14 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
+    <row r="101" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" t="s">
         <v>325</v>
       </c>
       <c r="D101" s="8" t="s">
@@ -8158,10 +8269,10 @@
       <c r="K101" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L101" s="10">
+      <c r="L101" s="9">
         <v>29108</v>
       </c>
-      <c r="M101" s="11">
+      <c r="M101" s="10">
         <v>35329</v>
       </c>
       <c r="N101" s="8" t="s">
@@ -8189,14 +8300,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
+    <row r="102" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C102" t="s">
         <v>328</v>
       </c>
       <c r="D102" s="8" t="s">
@@ -8223,10 +8334,10 @@
       <c r="K102" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L102" s="10">
+      <c r="L102" s="9">
         <v>29177</v>
       </c>
-      <c r="M102" s="11">
+      <c r="M102" s="10">
         <v>35875</v>
       </c>
       <c r="N102" s="8" t="s">
@@ -8254,14 +8365,14 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
+    <row r="103" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C103" t="s">
         <v>330</v>
       </c>
       <c r="D103" s="8" t="s">
@@ -8288,10 +8399,10 @@
       <c r="K103" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L103" s="10">
+      <c r="L103" s="9">
         <v>28957</v>
       </c>
-      <c r="M103" s="11">
+      <c r="M103" s="10">
         <v>35847</v>
       </c>
       <c r="N103" s="8" t="s">
@@ -8319,14 +8430,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
+    <row r="104" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C104" t="s">
         <v>332</v>
       </c>
       <c r="D104" s="8" t="s">
@@ -8353,10 +8464,10 @@
       <c r="K104" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L104" s="10">
+      <c r="L104" s="9">
         <v>27843</v>
       </c>
-      <c r="M104" s="11">
+      <c r="M104" s="10">
         <v>37124</v>
       </c>
       <c r="N104" s="8" t="s">
@@ -8384,14 +8495,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
+    <row r="105" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" t="s">
         <v>336</v>
       </c>
       <c r="D105" s="8" t="s">
@@ -8418,10 +8529,10 @@
       <c r="K105" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L105" s="10">
+      <c r="L105" s="9">
         <v>27182</v>
       </c>
-      <c r="M105" s="11">
+      <c r="M105" s="10">
         <v>37032</v>
       </c>
       <c r="N105" s="8" t="s">
@@ -8449,14 +8560,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
+    <row r="106" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" t="s">
         <v>339</v>
       </c>
       <c r="D106" s="8" t="s">
@@ -8483,10 +8594,10 @@
       <c r="K106" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L106" s="10">
+      <c r="L106" s="9">
         <v>30302</v>
       </c>
-      <c r="M106" s="11">
+      <c r="M106" s="10">
         <v>40544</v>
       </c>
       <c r="N106" s="8" t="s">
@@ -8514,14 +8625,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
+    <row r="107" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" t="s">
         <v>344</v>
       </c>
       <c r="D107" s="8" t="s">
@@ -8548,10 +8659,10 @@
       <c r="K107" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L107" s="10">
+      <c r="L107" s="9">
         <v>34192</v>
       </c>
-      <c r="M107" s="11">
+      <c r="M107" s="10">
         <v>43891</v>
       </c>
       <c r="N107" s="8" t="s">
@@ -8579,14 +8690,14 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
+    <row r="108" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" t="s">
         <v>347</v>
       </c>
       <c r="D108" s="8" t="s">
@@ -8613,10 +8724,10 @@
       <c r="K108" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L108" s="10">
+      <c r="L108" s="9">
         <v>35514</v>
       </c>
-      <c r="M108" s="11">
+      <c r="M108" s="10">
         <v>44515</v>
       </c>
       <c r="N108" s="8" t="s">
@@ -8644,14 +8755,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
+    <row r="109" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>108</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" t="s">
         <v>350</v>
       </c>
       <c r="D109" s="8" t="s">
@@ -8678,10 +8789,10 @@
       <c r="K109" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L109" s="10">
+      <c r="L109" s="9">
         <v>36557</v>
       </c>
-      <c r="M109" s="11">
+      <c r="M109" s="10">
         <v>44515</v>
       </c>
       <c r="N109" s="8" t="s">
@@ -8709,14 +8820,14 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
+    <row r="110" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C110" t="s">
         <v>353</v>
       </c>
       <c r="D110" s="8" t="s">
@@ -8743,10 +8854,10 @@
       <c r="K110" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L110" s="10">
+      <c r="L110" s="9">
         <v>35326</v>
       </c>
-      <c r="M110" s="11">
+      <c r="M110" s="10">
         <v>44515</v>
       </c>
       <c r="N110" s="8" t="s">
@@ -8774,14 +8885,14 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
+    <row r="111" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C111" t="s">
         <v>356</v>
       </c>
       <c r="D111" s="8" t="s">
@@ -8808,10 +8919,10 @@
       <c r="K111" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L111" s="10">
+      <c r="L111" s="9">
         <v>35009</v>
       </c>
-      <c r="M111" s="11">
+      <c r="M111" s="10">
         <v>44515</v>
       </c>
       <c r="N111" s="8" t="s">
@@ -8839,14 +8950,14 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
+    <row r="112" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C112" t="s">
         <v>359</v>
       </c>
       <c r="D112" s="8" t="s">
@@ -8873,10 +8984,10 @@
       <c r="K112" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L112" s="10">
+      <c r="L112" s="9">
         <v>35424</v>
       </c>
-      <c r="M112" s="12">
+      <c r="M112" s="11">
         <v>44515</v>
       </c>
       <c r="N112" s="8" t="s">
@@ -8904,14 +9015,14 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
+    <row r="113" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C113" t="s">
         <v>363</v>
       </c>
       <c r="D113" s="8" t="s">
@@ -8938,10 +9049,10 @@
       <c r="K113" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L113" s="10">
+      <c r="L113" s="9">
         <v>33765</v>
       </c>
-      <c r="M113" s="12">
+      <c r="M113" s="11">
         <v>44800</v>
       </c>
       <c r="N113" s="8" t="s">
@@ -8975,22 +9086,766 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="24">
+        <v>79</v>
+      </c>
+      <c r="D3" s="24">
+        <v>88</v>
+      </c>
+      <c r="E3" s="24">
+        <v>88</v>
+      </c>
+      <c r="F3" s="24">
+        <v>89</v>
+      </c>
+      <c r="G3" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="24">
+        <v>80</v>
+      </c>
+      <c r="D4" s="24">
+        <v>87</v>
+      </c>
+      <c r="E4" s="24">
+        <v>89</v>
+      </c>
+      <c r="F4" s="24">
+        <v>91</v>
+      </c>
+      <c r="G4" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="24">
+        <v>80</v>
+      </c>
+      <c r="D5" s="24">
+        <v>85</v>
+      </c>
+      <c r="E5" s="24">
+        <v>87</v>
+      </c>
+      <c r="F5" s="24">
+        <v>88</v>
+      </c>
+      <c r="G5" s="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22">
+        <v>4</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="24">
+        <v>79</v>
+      </c>
+      <c r="D6" s="24">
+        <v>90</v>
+      </c>
+      <c r="E6" s="24">
+        <v>86</v>
+      </c>
+      <c r="F6" s="24">
+        <v>90</v>
+      </c>
+      <c r="G6" s="24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="24">
+        <v>81</v>
+      </c>
+      <c r="D7" s="24">
+        <v>88</v>
+      </c>
+      <c r="E7" s="24">
+        <v>92</v>
+      </c>
+      <c r="F7" s="24">
+        <v>86</v>
+      </c>
+      <c r="G7" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="24">
+        <v>81</v>
+      </c>
+      <c r="D8" s="24">
+        <v>91</v>
+      </c>
+      <c r="E8" s="24">
+        <v>88</v>
+      </c>
+      <c r="F8" s="24">
+        <v>92</v>
+      </c>
+      <c r="G8" s="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="24">
+        <v>80</v>
+      </c>
+      <c r="D9" s="24">
+        <v>89</v>
+      </c>
+      <c r="E9" s="24">
+        <v>91</v>
+      </c>
+      <c r="F9" s="24">
+        <v>89</v>
+      </c>
+      <c r="G9" s="24">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22">
+        <v>8</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="24">
+        <v>79</v>
+      </c>
+      <c r="D10" s="24">
+        <v>85</v>
+      </c>
+      <c r="E10" s="24">
+        <v>89</v>
+      </c>
+      <c r="F10" s="24">
+        <v>91</v>
+      </c>
+      <c r="G10" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
+        <v>9</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="24">
+        <v>79</v>
+      </c>
+      <c r="D11" s="24">
+        <v>86</v>
+      </c>
+      <c r="E11" s="24">
+        <v>87</v>
+      </c>
+      <c r="F11" s="24">
+        <v>88</v>
+      </c>
+      <c r="G11" s="24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>10</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="24">
+        <v>80</v>
+      </c>
+      <c r="D12" s="24">
+        <v>88</v>
+      </c>
+      <c r="E12" s="24">
+        <v>90</v>
+      </c>
+      <c r="F12" s="24">
+        <v>87</v>
+      </c>
+      <c r="G12" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>11</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="24">
+        <v>78</v>
+      </c>
+      <c r="D13" s="24">
+        <v>86</v>
+      </c>
+      <c r="E13" s="24">
+        <v>86</v>
+      </c>
+      <c r="F13" s="24">
+        <v>90</v>
+      </c>
+      <c r="G13" s="24">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>12</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="24">
+        <v>78</v>
+      </c>
+      <c r="D14" s="24">
+        <v>90</v>
+      </c>
+      <c r="E14" s="24">
+        <v>90</v>
+      </c>
+      <c r="F14" s="24">
+        <v>86</v>
+      </c>
+      <c r="G14" s="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>13</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="24">
+        <v>85</v>
+      </c>
+      <c r="D15" s="24">
+        <v>86</v>
+      </c>
+      <c r="E15" s="24">
+        <v>92</v>
+      </c>
+      <c r="F15" s="24">
+        <v>92</v>
+      </c>
+      <c r="G15" s="24">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22">
+        <v>14</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="24">
+        <v>90</v>
+      </c>
+      <c r="D16" s="24">
+        <v>87</v>
+      </c>
+      <c r="E16" s="24">
+        <v>89</v>
+      </c>
+      <c r="F16" s="24">
+        <v>92</v>
+      </c>
+      <c r="G16" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
+        <v>15</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="24">
+        <v>85</v>
+      </c>
+      <c r="D17" s="24">
+        <v>91</v>
+      </c>
+      <c r="E17" s="24">
+        <v>92</v>
+      </c>
+      <c r="F17" s="24">
+        <v>88</v>
+      </c>
+      <c r="G17" s="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22">
+        <v>16</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="24">
+        <v>90</v>
+      </c>
+      <c r="D18" s="24">
+        <v>89</v>
+      </c>
+      <c r="E18" s="24">
+        <v>90</v>
+      </c>
+      <c r="F18" s="24">
+        <v>90</v>
+      </c>
+      <c r="G18" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22">
+        <v>17</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="24">
+        <v>90</v>
+      </c>
+      <c r="D19" s="24">
+        <v>86</v>
+      </c>
+      <c r="E19" s="24">
+        <v>88</v>
+      </c>
+      <c r="F19" s="24">
+        <v>86</v>
+      </c>
+      <c r="G19" s="24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22">
+        <v>18</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="24">
+        <v>87</v>
+      </c>
+      <c r="D20" s="24">
+        <v>88</v>
+      </c>
+      <c r="E20" s="24">
+        <v>91</v>
+      </c>
+      <c r="F20" s="24">
+        <v>92</v>
+      </c>
+      <c r="G20" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
+        <v>19</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="24">
+        <v>88</v>
+      </c>
+      <c r="D21" s="24">
+        <v>90</v>
+      </c>
+      <c r="E21" s="24">
+        <v>87</v>
+      </c>
+      <c r="F21" s="24">
+        <v>89</v>
+      </c>
+      <c r="G21" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="24">
+        <v>85</v>
+      </c>
+      <c r="D22" s="24">
+        <v>85</v>
+      </c>
+      <c r="E22" s="24">
+        <v>92</v>
+      </c>
+      <c r="F22" s="24">
+        <v>90</v>
+      </c>
+      <c r="G22" s="24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22">
+        <v>21</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="24">
+        <v>86</v>
+      </c>
+      <c r="D23" s="24">
+        <v>89</v>
+      </c>
+      <c r="E23" s="24">
+        <v>89</v>
+      </c>
+      <c r="F23" s="24">
+        <v>87</v>
+      </c>
+      <c r="G23" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22">
+        <v>22</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="24">
+        <v>89</v>
+      </c>
+      <c r="D24" s="24">
+        <v>87</v>
+      </c>
+      <c r="E24" s="24">
+        <v>90</v>
+      </c>
+      <c r="F24" s="24">
+        <v>88</v>
+      </c>
+      <c r="G24" s="24">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22">
+        <v>23</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="24">
+        <v>88</v>
+      </c>
+      <c r="D25" s="24">
+        <v>91</v>
+      </c>
+      <c r="E25" s="24">
+        <v>86</v>
+      </c>
+      <c r="F25" s="24">
+        <v>88</v>
+      </c>
+      <c r="G25" s="24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22">
+        <v>24</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="24">
+        <v>87</v>
+      </c>
+      <c r="D26" s="24">
+        <v>90</v>
+      </c>
+      <c r="E26" s="24">
+        <v>88</v>
+      </c>
+      <c r="F26" s="24">
+        <v>90</v>
+      </c>
+      <c r="G26" s="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22">
+        <v>25</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="24">
+        <v>86</v>
+      </c>
+      <c r="D27" s="24">
+        <v>88</v>
+      </c>
+      <c r="E27" s="24">
+        <v>90</v>
+      </c>
+      <c r="F27" s="24">
+        <v>92</v>
+      </c>
+      <c r="G27" s="24">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22">
+        <v>26</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="24">
+        <v>88</v>
+      </c>
+      <c r="D28" s="24">
+        <v>91</v>
+      </c>
+      <c r="E28" s="24">
+        <v>93</v>
+      </c>
+      <c r="F28" s="24">
+        <v>91</v>
+      </c>
+      <c r="G28" s="24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
+        <v>27</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="24">
+        <v>85</v>
+      </c>
+      <c r="D29" s="24">
+        <v>85</v>
+      </c>
+      <c r="E29" s="24">
+        <v>88</v>
+      </c>
+      <c r="F29" s="24">
+        <v>89</v>
+      </c>
+      <c r="G29" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22">
+        <v>28</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="24">
+        <v>85</v>
+      </c>
+      <c r="D30" s="24">
+        <v>90</v>
+      </c>
+      <c r="E30" s="24">
+        <v>87</v>
+      </c>
+      <c r="F30" s="24">
+        <v>90</v>
+      </c>
+      <c r="G30" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22">
+        <v>29</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="24">
+        <v>85</v>
+      </c>
+      <c r="D31" s="24">
+        <v>87</v>
+      </c>
+      <c r="E31" s="24">
+        <v>90</v>
+      </c>
+      <c r="F31" s="24">
+        <v>89</v>
+      </c>
+      <c r="G31" s="24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22">
+        <v>30</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="24">
+        <v>79</v>
+      </c>
+      <c r="D32" s="24">
+        <v>88</v>
+      </c>
+      <c r="E32" s="24">
+        <v>88</v>
+      </c>
+      <c r="F32" s="24">
+        <v>89</v>
+      </c>
+      <c r="G32" s="24">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>

</xml_diff>